<commit_message>
Monocity docx prep corr.
</commit_message>
<xml_diff>
--- a/migforecasting/cities17-18/0/d2.xlsx
+++ b/migforecasting/cities17-18/0/d2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="220">
   <si>
     <t>2017</t>
   </si>
@@ -722,6 +722,9 @@
 на земельных участках, предназначенных для ведения садоводства.
 12) За 2017, 2018 гг. – по сопоставимому кругу организаций, за 2019 г. – по отношению к данным, сложившимся в соответствующем периоде прошлого года, 
 без учета демографии за отчетный год.</t>
+  </si>
+  <si>
+    <t>Майкоп</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,14 +1113,17 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>219</v>
+      </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>219</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1128,13 +1134,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>